<commit_message>
push to continue on laptop
</commit_message>
<xml_diff>
--- a/data/02_data_extraction/data_extraction_UnpublishedThesis.xlsx
+++ b/data/02_data_extraction/data_extraction_UnpublishedThesis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyadimri/Library/CloudStorage/Dropbox/GitHub_Repo/GNM_Analysis/data/02_data_extraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyadimri/Library/CloudStorage/Dropbox/GitHub_Repo/Green_Nest_Material/data/02_data_extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EE0C9B-9CB6-BD4D-BCBC-01BBCE24914F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131BC2DA-DC5E-714F-B59A-87E7A91E1F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33220" yWindow="500" windowWidth="43580" windowHeight="21100" xr2:uid="{2338411D-A035-6640-9B5F-097AD98E903E}"/>
+    <workbookView xWindow="33220" yWindow="500" windowWidth="43600" windowHeight="20120" xr2:uid="{2338411D-A035-6640-9B5F-097AD98E903E}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DCDDD25-569C-114E-BA1C-CFE63559CC31}">
   <dimension ref="A1:AX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1173,7 +1173,7 @@
         <v>114</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -1325,7 +1325,7 @@
         <v>114</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O3">
         <v>1</v>
@@ -1477,7 +1477,7 @@
         <v>114</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -1629,7 +1629,7 @@
         <v>114</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -1781,7 +1781,7 @@
         <v>114</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -1933,7 +1933,7 @@
         <v>114</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -2085,7 +2085,7 @@
         <v>114</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -2237,7 +2237,7 @@
         <v>114</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O9">
         <v>1</v>
@@ -2389,7 +2389,7 @@
         <v>114</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10">
         <v>1</v>

</xml_diff>